<commit_message>
pouvoir / perisprit / esprit finish
</commit_message>
<xml_diff>
--- a/Cabinet des murmures/ressources/Cabinet schema.xlsx
+++ b/Cabinet des murmures/ressources/Cabinet schema.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cabinet" sheetId="1" r:id="rId1"/>
     <sheet name="Esprit" sheetId="2" r:id="rId2"/>
     <sheet name="Corps" sheetId="4" r:id="rId3"/>
     <sheet name="Arme" sheetId="5" r:id="rId4"/>
+    <sheet name="pouvoir" sheetId="6" r:id="rId5"/>
+    <sheet name="perisprit" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>XP</t>
   </si>
@@ -78,6 +80,18 @@
   <si>
     <t>cadence</t>
   </si>
+  <si>
+    <t>Niveau</t>
+  </si>
+  <si>
+    <t>S.</t>
+  </si>
+  <si>
+    <t>P.</t>
+  </si>
+  <si>
+    <t>C.</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,8 +258,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -407,11 +433,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,6 +500,174 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,174 +792,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -780,6 +821,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,23 +845,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -825,24 +884,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,6 +929,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1211,419 +1264,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="A1" s="88"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="103"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="64"/>
+      <c r="A2" s="91"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="120"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="67"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="123"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="67"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="123"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="123"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="67"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="123"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="67"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="123"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="67"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="123"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="67"/>
-      <c r="L10" s="29"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="122"/>
+      <c r="J10" s="123"/>
+      <c r="L10" s="85"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="67"/>
-      <c r="L11" s="30"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="123"/>
+      <c r="L11" s="86"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="70"/>
-      <c r="L12" s="30"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="125"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="126"/>
+      <c r="L12" s="86"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="74"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="100"/>
-      <c r="L13" s="30"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="58"/>
+      <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="77"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="103"/>
-      <c r="L14" s="30"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="61"/>
+      <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="106"/>
-      <c r="L15" s="30"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="64"/>
+      <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="104"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="106"/>
-      <c r="L16" s="30"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="64"/>
+      <c r="L16" s="86"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="106"/>
-      <c r="L17" s="30"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="64"/>
+      <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="106"/>
-      <c r="L18" s="30"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="64"/>
+      <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="80"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="105"/>
-      <c r="J19" s="106"/>
-      <c r="L19" s="31"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="64"/>
+      <c r="L19" s="87"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="83"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="109"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="67"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="86"/>
-      <c r="B21" s="87"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="124"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="111"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="69"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="89"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="124"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="113"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="71"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="92"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="124"/>
-      <c r="I23" s="114"/>
-      <c r="J23" s="115"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="73"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="124"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="115"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="124"/>
-      <c r="I25" s="114"/>
-      <c r="J25" s="115"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
-      <c r="B26" s="93"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="124"/>
-      <c r="I26" s="114"/>
-      <c r="J26" s="115"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="73"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="92"/>
-      <c r="B27" s="93"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="93"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="124"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="117"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="75"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
-      <c r="B28" s="93"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="93"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="124"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="83"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="92"/>
-      <c r="B29" s="93"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="93"/>
-      <c r="F29" s="93"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="124"/>
-      <c r="I29" s="126"/>
-      <c r="J29" s="126"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="84"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="124"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="119"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="77"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="92"/>
-      <c r="B31" s="93"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="124"/>
-      <c r="I31" s="120"/>
-      <c r="J31" s="121"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="79"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
-      <c r="B32" s="93"/>
-      <c r="C32" s="93"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="124"/>
-      <c r="I32" s="120"/>
-      <c r="J32" s="121"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="78"/>
+      <c r="J32" s="79"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="95"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="124"/>
-      <c r="I33" s="122"/>
-      <c r="J33" s="123"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="81"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="71"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="73"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="L10:L19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E5"/>
+    <mergeCell ref="F1:F20"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="G2:J12"/>
+    <mergeCell ref="B7:B12"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E20"/>
@@ -1636,18 +1701,6 @@
     <mergeCell ref="I30:J33"/>
     <mergeCell ref="H21:H33"/>
     <mergeCell ref="I28:J29"/>
-    <mergeCell ref="L10:L19"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E5"/>
-    <mergeCell ref="F1:F20"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="G2:J12"/>
-    <mergeCell ref="B7:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1658,7 +1711,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43:J43"/>
+      <selection activeCell="A20" sqref="A20:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,19 +1793,19 @@
       <c r="M4" s="135"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="139"/>
-      <c r="B5" s="140"/>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="140"/>
-      <c r="H5" s="140"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="140"/>
-      <c r="M5" s="141"/>
+      <c r="A5" s="136"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="137"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="137"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="138"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="127" t="s">
@@ -1890,21 +1943,21 @@
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="138"/>
+      <c r="B14" s="142"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="143"/>
       <c r="G14" s="24"/>
-      <c r="H14" s="139"/>
-      <c r="I14" s="140"/>
-      <c r="J14" s="140"/>
-      <c r="K14" s="140"/>
-      <c r="L14" s="140"/>
-      <c r="M14" s="141"/>
+      <c r="H14" s="136"/>
+      <c r="I14" s="137"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="137"/>
+      <c r="L14" s="137"/>
+      <c r="M14" s="138"/>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1958,12 +2011,12 @@
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="139"/>
-      <c r="B18" s="140"/>
-      <c r="C18" s="140"/>
-      <c r="D18" s="140"/>
-      <c r="E18" s="140"/>
-      <c r="F18" s="141"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="138"/>
       <c r="G18" s="25"/>
       <c r="H18" s="133"/>
       <c r="I18" s="134"/>
@@ -1974,14 +2027,14 @@
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="144"/>
-      <c r="C19" s="144"/>
-      <c r="D19" s="144"/>
-      <c r="E19" s="144"/>
-      <c r="F19" s="144"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
+      <c r="F19" s="140"/>
       <c r="G19" s="128"/>
       <c r="H19" s="128"/>
       <c r="I19" s="128"/>
@@ -2070,19 +2123,19 @@
       <c r="M24" s="135"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="139"/>
-      <c r="B25" s="140"/>
-      <c r="C25" s="140"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="139"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="140"/>
-      <c r="I25" s="141"/>
-      <c r="J25" s="139"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="140"/>
-      <c r="M25" s="141"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="138"/>
+      <c r="J25" s="136"/>
+      <c r="K25" s="137"/>
+      <c r="L25" s="137"/>
+      <c r="M25" s="138"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="127" t="s">
@@ -2096,7 +2149,7 @@
       <c r="G26" s="128"/>
       <c r="H26" s="128"/>
       <c r="I26" s="128"/>
-      <c r="J26" s="142"/>
+      <c r="J26" s="144"/>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
@@ -2119,16 +2172,16 @@
       <c r="M27" s="132"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="139"/>
-      <c r="B28" s="140"/>
-      <c r="C28" s="140"/>
-      <c r="D28" s="140"/>
-      <c r="E28" s="140"/>
-      <c r="F28" s="140"/>
-      <c r="G28" s="140"/>
-      <c r="H28" s="140"/>
-      <c r="I28" s="140"/>
-      <c r="J28" s="140"/>
+      <c r="A28" s="136"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="137"/>
+      <c r="H28" s="137"/>
+      <c r="I28" s="137"/>
+      <c r="J28" s="137"/>
       <c r="K28" s="23"/>
       <c r="L28" s="133"/>
       <c r="M28" s="135"/>
@@ -2166,19 +2219,19 @@
       <c r="M30" s="135"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="139"/>
-      <c r="B31" s="140"/>
-      <c r="C31" s="140"/>
-      <c r="D31" s="140"/>
-      <c r="E31" s="140"/>
-      <c r="F31" s="140"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="140"/>
-      <c r="I31" s="140"/>
-      <c r="J31" s="140"/>
+      <c r="A31" s="136"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="137"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="137"/>
+      <c r="J31" s="137"/>
       <c r="K31" s="23"/>
-      <c r="L31" s="139"/>
-      <c r="M31" s="141"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="138"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
@@ -2267,11 +2320,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A27:J28"/>
-    <mergeCell ref="A29:J29"/>
     <mergeCell ref="A30:J31"/>
     <mergeCell ref="L27:M31"/>
     <mergeCell ref="A11:F11"/>
@@ -2283,11 +2331,16 @@
     <mergeCell ref="H15:M15"/>
     <mergeCell ref="H16:M18"/>
     <mergeCell ref="H12:M14"/>
-    <mergeCell ref="E6:M6"/>
     <mergeCell ref="A12:F13"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A15:F18"/>
     <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A27:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="E6:M6"/>
     <mergeCell ref="J7:M10"/>
     <mergeCell ref="A7:C10"/>
     <mergeCell ref="E7:H10"/>
@@ -2323,90 +2376,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="149"/>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="52"/>
+      <c r="A1" s="155"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="108"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="44"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="100"/>
       <c r="J2" s="13"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="44"/>
+      <c r="A3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="100"/>
       <c r="J3" s="16"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="44"/>
+      <c r="A4" s="94"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="100"/>
       <c r="J4" s="16"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="44"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="100"/>
       <c r="J5" s="16"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="147"/>
-      <c r="B6" s="148"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="44"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="154"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="154"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="100"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -2415,13 +2468,13 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="157"/>
       <c r="B7" s="158"/>
-      <c r="C7" s="48"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="163"/>
       <c r="E7" s="164"/>
-      <c r="F7" s="48"/>
+      <c r="F7" s="104"/>
       <c r="G7" s="169"/>
       <c r="H7" s="170"/>
-      <c r="I7" s="44"/>
+      <c r="I7" s="100"/>
       <c r="J7" s="16"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
@@ -2430,13 +2483,13 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="159"/>
       <c r="B8" s="160"/>
-      <c r="C8" s="49"/>
+      <c r="C8" s="105"/>
       <c r="D8" s="165"/>
       <c r="E8" s="166"/>
-      <c r="F8" s="49"/>
+      <c r="F8" s="105"/>
       <c r="G8" s="169"/>
       <c r="H8" s="170"/>
-      <c r="I8" s="44"/>
+      <c r="I8" s="100"/>
       <c r="J8" s="16"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
@@ -2445,13 +2498,13 @@
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="159"/>
       <c r="B9" s="160"/>
-      <c r="C9" s="49"/>
+      <c r="C9" s="105"/>
       <c r="D9" s="165"/>
       <c r="E9" s="166"/>
-      <c r="F9" s="49"/>
+      <c r="F9" s="105"/>
       <c r="G9" s="169"/>
       <c r="H9" s="170"/>
-      <c r="I9" s="44"/>
+      <c r="I9" s="100"/>
       <c r="J9" s="16"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2460,50 +2513,50 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="159"/>
       <c r="B10" s="160"/>
-      <c r="C10" s="49"/>
+      <c r="C10" s="105"/>
       <c r="D10" s="165"/>
       <c r="E10" s="166"/>
-      <c r="F10" s="49"/>
+      <c r="F10" s="105"/>
       <c r="G10" s="169"/>
       <c r="H10" s="170"/>
-      <c r="I10" s="44"/>
+      <c r="I10" s="100"/>
       <c r="J10" s="16"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="17"/>
-      <c r="O10" s="29"/>
+      <c r="O10" s="85"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="161"/>
       <c r="B11" s="162"/>
-      <c r="C11" s="49"/>
+      <c r="C11" s="105"/>
       <c r="D11" s="167"/>
       <c r="E11" s="168"/>
-      <c r="F11" s="49"/>
+      <c r="F11" s="105"/>
       <c r="G11" s="169"/>
       <c r="H11" s="170"/>
-      <c r="I11" s="44"/>
+      <c r="I11" s="100"/>
       <c r="J11" s="16"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="17"/>
-      <c r="O11" s="30"/>
+      <c r="O11" s="86"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="74"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="1"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="152"/>
-      <c r="I12" s="44"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="100"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="17"/>
-      <c r="O12" s="30"/>
+      <c r="O12" s="86"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -2512,14 +2565,14 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="155"/>
-      <c r="H13" s="156"/>
-      <c r="I13" s="44"/>
+      <c r="G13" s="149"/>
+      <c r="H13" s="150"/>
+      <c r="I13" s="100"/>
       <c r="J13" s="16"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="17"/>
-      <c r="O13" s="30"/>
+      <c r="O13" s="86"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -2528,14 +2581,14 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="44"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="100"/>
       <c r="J14" s="16"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="30"/>
+      <c r="O14" s="86"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -2544,14 +2597,14 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="44"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="100"/>
       <c r="J15" s="16"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="17"/>
-      <c r="O15" s="30"/>
+      <c r="O15" s="86"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -2562,14 +2615,14 @@
         <v>9</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="104"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="44"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="100"/>
       <c r="J16" s="16"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="17"/>
-      <c r="O16" s="30"/>
+      <c r="O16" s="86"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -2578,14 +2631,14 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="146"/>
-      <c r="I17" s="44"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="152"/>
+      <c r="I17" s="100"/>
       <c r="J17" s="16"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="17"/>
-      <c r="O17" s="30"/>
+      <c r="O17" s="86"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
@@ -2594,14 +2647,14 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="44"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="100"/>
       <c r="J18" s="16"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="17"/>
-      <c r="O18" s="31"/>
+      <c r="O18" s="87"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -2610,9 +2663,9 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="44"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="100"/>
       <c r="J19" s="16"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -2625,8 +2678,8 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="95"/>
       <c r="I20" s="2"/>
       <c r="J20" s="16"/>
       <c r="K20" s="12"/>
@@ -2649,14 +2702,14 @@
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="11"/>
       <c r="J22" s="16"/>
       <c r="K22" s="12"/>
@@ -2664,14 +2717,14 @@
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="92"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
       <c r="I23" s="11"/>
       <c r="J23" s="16"/>
       <c r="K23" s="12"/>
@@ -2679,14 +2732,14 @@
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
-      <c r="B24" s="93"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
       <c r="I24" s="11"/>
       <c r="J24" s="16"/>
       <c r="K24" s="12"/>
@@ -2694,14 +2747,14 @@
       <c r="M24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
       <c r="I25" s="11"/>
       <c r="J25" s="16"/>
       <c r="K25" s="12"/>
@@ -2709,14 +2762,14 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
-      <c r="B26" s="93"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="93"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
       <c r="I26" s="11"/>
       <c r="J26" s="16"/>
       <c r="K26" s="12"/>
@@ -2724,14 +2777,14 @@
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="153"/>
-      <c r="B27" s="154"/>
-      <c r="C27" s="154"/>
-      <c r="D27" s="154"/>
-      <c r="E27" s="154"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="154"/>
-      <c r="H27" s="154"/>
+      <c r="A27" s="147"/>
+      <c r="B27" s="148"/>
+      <c r="C27" s="148"/>
+      <c r="D27" s="148"/>
+      <c r="E27" s="148"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="148"/>
+      <c r="H27" s="148"/>
       <c r="I27" s="11"/>
       <c r="J27" s="16"/>
       <c r="K27" s="12"/>
@@ -2739,14 +2792,14 @@
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
       <c r="I28" s="11"/>
       <c r="J28" s="16"/>
       <c r="K28" s="12"/>
@@ -2754,14 +2807,14 @@
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
       <c r="I29" s="11"/>
       <c r="J29" s="16"/>
       <c r="K29" s="12"/>
@@ -2769,14 +2822,14 @@
       <c r="M29" s="17"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
       <c r="I30" s="11"/>
       <c r="J30" s="16"/>
       <c r="K30" s="12"/>
@@ -2784,14 +2837,14 @@
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="80"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="81"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
       <c r="I31" s="11"/>
       <c r="J31" s="16"/>
       <c r="K31" s="12"/>
@@ -2799,14 +2852,14 @@
       <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
       <c r="I32" s="11"/>
       <c r="J32" s="16"/>
       <c r="K32" s="12"/>
@@ -2814,14 +2867,14 @@
       <c r="M32" s="17"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
       <c r="I33" s="11"/>
       <c r="J33" s="18"/>
       <c r="K33" s="19"/>
@@ -2830,21 +2883,13 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="71"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="73"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A22:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H33"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H16"/>
     <mergeCell ref="O10:O18"/>
     <mergeCell ref="G18:H20"/>
     <mergeCell ref="G17:H17"/>
@@ -2858,6 +2903,14 @@
     <mergeCell ref="A7:B11"/>
     <mergeCell ref="D7:E11"/>
     <mergeCell ref="G7:H11"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A22:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H33"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2868,7 +2921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -3024,4 +3077,424 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="3" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" customWidth="1"/>
+    <col min="18" max="18" width="3.28515625" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" customWidth="1"/>
+    <col min="23" max="23" width="4.28515625" customWidth="1"/>
+    <col min="24" max="24" width="3.7109375" customWidth="1"/>
+    <col min="25" max="25" width="4" customWidth="1"/>
+    <col min="26" max="26" width="4.5703125" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" customWidth="1"/>
+    <col min="28" max="28" width="3.140625" customWidth="1"/>
+    <col min="29" max="29" width="5.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="173" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="173" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="172"/>
+      <c r="N1" s="172"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="173" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="172"/>
+      <c r="X1" s="172"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D2" s="175" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="175"/>
+      <c r="G2" s="176" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="176" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="177"/>
+      <c r="N2" s="175" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="175"/>
+      <c r="Q2" s="176" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="176" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="177"/>
+      <c r="X2" s="175" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="175"/>
+      <c r="AA2" s="176" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC2" s="176" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="174"/>
+      <c r="B3" s="174"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
+      <c r="G3" s="176"/>
+      <c r="I3" s="176"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="174"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="Q3" s="176"/>
+      <c r="S3" s="176"/>
+      <c r="T3" s="177"/>
+      <c r="U3" s="174"/>
+      <c r="V3" s="174"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="AA3" s="176"/>
+      <c r="AC3" s="176"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="174"/>
+      <c r="B4" s="174"/>
+      <c r="D4" s="175"/>
+      <c r="E4" s="175"/>
+      <c r="G4" s="176"/>
+      <c r="I4" s="176"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="174"/>
+      <c r="L4" s="174"/>
+      <c r="N4" s="175"/>
+      <c r="O4" s="175"/>
+      <c r="Q4" s="176"/>
+      <c r="S4" s="176"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="174"/>
+      <c r="V4" s="174"/>
+      <c r="X4" s="175"/>
+      <c r="Y4" s="175"/>
+      <c r="AA4" s="176"/>
+      <c r="AC4" s="176"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="174"/>
+      <c r="B5" s="174"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
+      <c r="G5" s="176"/>
+      <c r="I5" s="176"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="174"/>
+      <c r="N5" s="175"/>
+      <c r="O5" s="175"/>
+      <c r="Q5" s="176"/>
+      <c r="S5" s="176"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="174"/>
+      <c r="V5" s="174"/>
+      <c r="X5" s="175"/>
+      <c r="Y5" s="175"/>
+      <c r="AA5" s="176"/>
+      <c r="AC5" s="176"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>13</v>
+      </c>
+      <c r="N7">
+        <v>14</v>
+      </c>
+      <c r="O7">
+        <v>15</v>
+      </c>
+      <c r="P7">
+        <v>16</v>
+      </c>
+      <c r="Q7">
+        <v>17</v>
+      </c>
+      <c r="R7">
+        <v>18</v>
+      </c>
+      <c r="S7">
+        <v>19</v>
+      </c>
+      <c r="T7">
+        <v>20</v>
+      </c>
+      <c r="U7">
+        <v>21</v>
+      </c>
+      <c r="V7">
+        <v>22</v>
+      </c>
+      <c r="W7">
+        <v>23</v>
+      </c>
+      <c r="X7">
+        <v>24</v>
+      </c>
+      <c r="Y7">
+        <v>25</v>
+      </c>
+      <c r="Z7">
+        <v>26</v>
+      </c>
+      <c r="AA7">
+        <v>27</v>
+      </c>
+      <c r="AB7">
+        <v>28</v>
+      </c>
+      <c r="AC7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>110</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>110</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>20</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>40</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>40</v>
+      </c>
+      <c r="T9">
+        <v>15</v>
+      </c>
+      <c r="U9">
+        <v>110</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9">
+        <v>5</v>
+      </c>
+      <c r="X9">
+        <v>20</v>
+      </c>
+      <c r="Y9">
+        <v>20</v>
+      </c>
+      <c r="Z9">
+        <v>5</v>
+      </c>
+      <c r="AA9">
+        <v>40</v>
+      </c>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AC9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>760</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+      <c r="I3">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>410</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
final qualite et resized arbre
</commit_message>
<xml_diff>
--- a/Cabinet des murmures/ressources/Cabinet schema.xlsx
+++ b/Cabinet des murmures/ressources/Cabinet schema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cabinet" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Arme" sheetId="5" r:id="rId4"/>
     <sheet name="pouvoir" sheetId="6" r:id="rId5"/>
     <sheet name="perisprit" sheetId="7" r:id="rId6"/>
+    <sheet name="arbre" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -452,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -500,6 +501,135 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,131 +798,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -803,39 +831,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,6 +852,66 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -866,81 +930,19 @@
     <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1264,419 +1266,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="88"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="103"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="91"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="120"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="67"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="123"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="123"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="70"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="97"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="121"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
-      <c r="J5" s="123"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="70"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="106"/>
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="123"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="70"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="109"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="123"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="70"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="121"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="123"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="110"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="116"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="121"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
-      <c r="J9" s="123"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="122"/>
-      <c r="I10" s="122"/>
-      <c r="J10" s="123"/>
-      <c r="L10" s="85"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="L10" s="32"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="121"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="122"/>
-      <c r="J11" s="123"/>
-      <c r="L11" s="86"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="70"/>
+      <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="111"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="125"/>
-      <c r="I12" s="125"/>
-      <c r="J12" s="126"/>
-      <c r="L12" s="86"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="73"/>
+      <c r="L12" s="33"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="58"/>
-      <c r="L13" s="86"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="103"/>
+      <c r="L13" s="33"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="61"/>
-      <c r="L14" s="86"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="106"/>
+      <c r="L14" s="33"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="64"/>
-      <c r="L15" s="86"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="108"/>
+      <c r="J15" s="109"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="64"/>
-      <c r="L16" s="86"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="109"/>
+      <c r="L16" s="33"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="64"/>
-      <c r="L17" s="86"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="109"/>
+      <c r="L17" s="33"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="64"/>
-      <c r="L18" s="86"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="109"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="64"/>
-      <c r="L19" s="87"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="109"/>
+      <c r="L19" s="34"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="41"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="67"/>
+      <c r="A20" s="86"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="112"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="69"/>
+      <c r="A21" s="89"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="114"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="93"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="116"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="73"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="118"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="73"/>
+      <c r="A24" s="95"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="117"/>
+      <c r="J24" s="118"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="73"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="127"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="118"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
+      <c r="A26" s="95"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="127"/>
+      <c r="I26" s="117"/>
+      <c r="J26" s="118"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="75"/>
+      <c r="A27" s="95"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="127"/>
+      <c r="I27" s="119"/>
+      <c r="J27" s="120"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
+      <c r="A28" s="95"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="127"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="82"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="127"/>
+      <c r="I29" s="129"/>
+      <c r="J29" s="129"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="82"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="77"/>
+      <c r="A30" s="95"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="127"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="122"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="79"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="96"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="127"/>
+      <c r="I31" s="123"/>
+      <c r="J31" s="124"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="79"/>
+      <c r="A32" s="95"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="127"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="124"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="82"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="81"/>
+      <c r="A33" s="98"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="100"/>
+      <c r="H33" s="127"/>
+      <c r="I33" s="125"/>
+      <c r="J33" s="126"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="31"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:G33"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J27"/>
+    <mergeCell ref="I30:J33"/>
+    <mergeCell ref="H21:H33"/>
+    <mergeCell ref="I28:J29"/>
     <mergeCell ref="L10:L19"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E5"/>
@@ -1689,18 +1703,6 @@
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="G2:J12"/>
     <mergeCell ref="B7:B12"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:G33"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J27"/>
-    <mergeCell ref="I30:J33"/>
-    <mergeCell ref="H21:H33"/>
-    <mergeCell ref="I28:J29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1731,21 +1733,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="129"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="140"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="130"/>
@@ -1760,154 +1762,154 @@
       <c r="J2" s="131"/>
       <c r="K2" s="131"/>
       <c r="L2" s="131"/>
-      <c r="M2" s="132"/>
+      <c r="M2" s="134"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="133"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="135"/>
+      <c r="A3" s="135"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="136"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="133"/>
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="134"/>
-      <c r="M4" s="135"/>
+      <c r="A4" s="135"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
+      <c r="M4" s="136"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="136"/>
-      <c r="B5" s="137"/>
-      <c r="C5" s="137"/>
-      <c r="D5" s="137"/>
-      <c r="E5" s="137"/>
-      <c r="F5" s="137"/>
-      <c r="G5" s="137"/>
-      <c r="H5" s="137"/>
-      <c r="I5" s="137"/>
-      <c r="J5" s="137"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="137"/>
-      <c r="M5" s="138"/>
+      <c r="A5" s="132"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="133"/>
+      <c r="D5" s="133"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="133"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="137"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="127" t="s">
+      <c r="A6" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="128"/>
-      <c r="C6" s="129"/>
+      <c r="B6" s="139"/>
+      <c r="C6" s="140"/>
       <c r="D6" s="24"/>
-      <c r="E6" s="127" t="s">
+      <c r="E6" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="129"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="139"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="139"/>
+      <c r="L6" s="139"/>
+      <c r="M6" s="140"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="130"/>
       <c r="B7" s="131"/>
-      <c r="C7" s="132"/>
+      <c r="C7" s="134"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="143"/>
+      <c r="G7" s="143"/>
+      <c r="H7" s="136"/>
       <c r="I7" s="24"/>
-      <c r="J7" s="133"/>
-      <c r="K7" s="134"/>
-      <c r="L7" s="134"/>
-      <c r="M7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="143"/>
+      <c r="L7" s="143"/>
+      <c r="M7" s="136"/>
       <c r="O7" s="26"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
-      <c r="C8" s="135"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="136"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="135"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="136"/>
       <c r="I8" s="24"/>
-      <c r="J8" s="133"/>
-      <c r="K8" s="134"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="135"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="143"/>
+      <c r="L8" s="143"/>
+      <c r="M8" s="136"/>
       <c r="O8" s="27"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
-      <c r="B9" s="134"/>
-      <c r="C9" s="135"/>
+      <c r="A9" s="135"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="136"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="135"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="136"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="133"/>
-      <c r="K9" s="134"/>
-      <c r="L9" s="134"/>
-      <c r="M9" s="135"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="143"/>
+      <c r="L9" s="143"/>
+      <c r="M9" s="136"/>
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
-      <c r="B10" s="134"/>
-      <c r="C10" s="135"/>
+      <c r="A10" s="135"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="136"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="135"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="143"/>
+      <c r="H10" s="136"/>
       <c r="I10" s="24"/>
-      <c r="J10" s="133"/>
-      <c r="K10" s="134"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="135"/>
+      <c r="J10" s="135"/>
+      <c r="K10" s="143"/>
+      <c r="L10" s="143"/>
+      <c r="M10" s="136"/>
       <c r="O10" s="27"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="127" t="s">
+      <c r="A11" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="128"/>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="129"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="140"/>
       <c r="G11" s="24"/>
-      <c r="H11" s="127" t="s">
+      <c r="H11" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="128"/>
-      <c r="J11" s="128"/>
-      <c r="K11" s="128"/>
-      <c r="L11" s="128"/>
-      <c r="M11" s="129"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="139"/>
+      <c r="L11" s="139"/>
+      <c r="M11" s="140"/>
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1916,48 +1918,48 @@
       <c r="C12" s="131"/>
       <c r="D12" s="131"/>
       <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="F12" s="134"/>
       <c r="G12" s="24"/>
       <c r="H12" s="130"/>
       <c r="I12" s="131"/>
       <c r="J12" s="131"/>
       <c r="K12" s="131"/>
       <c r="L12" s="131"/>
-      <c r="M12" s="132"/>
+      <c r="M12" s="134"/>
       <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="133"/>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="135"/>
+      <c r="A13" s="135"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="143"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="136"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="134"/>
-      <c r="K13" s="134"/>
-      <c r="L13" s="134"/>
-      <c r="M13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="143"/>
+      <c r="J13" s="143"/>
+      <c r="K13" s="143"/>
+      <c r="L13" s="143"/>
+      <c r="M13" s="136"/>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="141" t="s">
+      <c r="A14" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="142"/>
-      <c r="C14" s="142"/>
-      <c r="D14" s="142"/>
-      <c r="E14" s="142"/>
-      <c r="F14" s="143"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="145"/>
+      <c r="E14" s="145"/>
+      <c r="F14" s="146"/>
       <c r="G14" s="24"/>
-      <c r="H14" s="136"/>
-      <c r="I14" s="137"/>
-      <c r="J14" s="137"/>
-      <c r="K14" s="137"/>
-      <c r="L14" s="137"/>
-      <c r="M14" s="138"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="133"/>
+      <c r="M14" s="137"/>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1966,190 +1968,190 @@
       <c r="C15" s="131"/>
       <c r="D15" s="131"/>
       <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="F15" s="134"/>
       <c r="G15" s="25"/>
-      <c r="H15" s="127" t="s">
+      <c r="H15" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="128"/>
-      <c r="J15" s="128"/>
-      <c r="K15" s="128"/>
-      <c r="L15" s="128"/>
-      <c r="M15" s="129"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="139"/>
+      <c r="L15" s="139"/>
+      <c r="M15" s="140"/>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="133"/>
-      <c r="B16" s="134"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="135"/>
+      <c r="A16" s="135"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="143"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="136"/>
       <c r="G16" s="25"/>
       <c r="H16" s="130"/>
       <c r="I16" s="131"/>
       <c r="J16" s="131"/>
       <c r="K16" s="131"/>
       <c r="L16" s="131"/>
-      <c r="M16" s="132"/>
+      <c r="M16" s="134"/>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="133"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="135"/>
+      <c r="A17" s="135"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="143"/>
+      <c r="E17" s="143"/>
+      <c r="F17" s="136"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="134"/>
-      <c r="J17" s="134"/>
-      <c r="K17" s="134"/>
-      <c r="L17" s="134"/>
-      <c r="M17" s="135"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="143"/>
+      <c r="J17" s="143"/>
+      <c r="K17" s="143"/>
+      <c r="L17" s="143"/>
+      <c r="M17" s="136"/>
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="137"/>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="138"/>
+      <c r="A18" s="132"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="137"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="134"/>
-      <c r="K18" s="134"/>
-      <c r="L18" s="134"/>
-      <c r="M18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="143"/>
+      <c r="J18" s="143"/>
+      <c r="K18" s="143"/>
+      <c r="L18" s="143"/>
+      <c r="M18" s="136"/>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="139" t="s">
+      <c r="A19" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="140"/>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="128"/>
-      <c r="K19" s="128"/>
-      <c r="L19" s="128"/>
-      <c r="M19" s="129"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="142"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="139"/>
+      <c r="K19" s="139"/>
+      <c r="L19" s="139"/>
+      <c r="M19" s="140"/>
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="130"/>
       <c r="B20" s="131"/>
       <c r="C20" s="131"/>
-      <c r="D20" s="132"/>
+      <c r="D20" s="134"/>
       <c r="E20" s="130"/>
       <c r="F20" s="131"/>
       <c r="G20" s="131"/>
       <c r="H20" s="131"/>
-      <c r="I20" s="132"/>
+      <c r="I20" s="134"/>
       <c r="J20" s="130"/>
       <c r="K20" s="131"/>
       <c r="L20" s="131"/>
-      <c r="M20" s="132"/>
+      <c r="M20" s="134"/>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="133"/>
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="133"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
-      <c r="H21" s="134"/>
-      <c r="I21" s="135"/>
-      <c r="J21" s="133"/>
-      <c r="K21" s="134"/>
-      <c r="L21" s="134"/>
-      <c r="M21" s="135"/>
+      <c r="A21" s="135"/>
+      <c r="B21" s="143"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="135"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="143"/>
+      <c r="H21" s="143"/>
+      <c r="I21" s="136"/>
+      <c r="J21" s="135"/>
+      <c r="K21" s="143"/>
+      <c r="L21" s="143"/>
+      <c r="M21" s="136"/>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="133"/>
-      <c r="B22" s="134"/>
-      <c r="C22" s="134"/>
-      <c r="D22" s="135"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="134"/>
-      <c r="I22" s="135"/>
-      <c r="J22" s="133"/>
-      <c r="K22" s="134"/>
-      <c r="L22" s="134"/>
-      <c r="M22" s="135"/>
+      <c r="A22" s="135"/>
+      <c r="B22" s="143"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="143"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="135"/>
+      <c r="K22" s="143"/>
+      <c r="L22" s="143"/>
+      <c r="M22" s="136"/>
       <c r="O22" s="28"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="133"/>
-      <c r="B23" s="134"/>
-      <c r="C23" s="134"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="134"/>
-      <c r="I23" s="135"/>
-      <c r="J23" s="133"/>
-      <c r="K23" s="134"/>
-      <c r="L23" s="134"/>
-      <c r="M23" s="135"/>
+      <c r="A23" s="135"/>
+      <c r="B23" s="143"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="136"/>
+      <c r="J23" s="135"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="136"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="133"/>
-      <c r="B24" s="134"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="135"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="134"/>
-      <c r="I24" s="135"/>
-      <c r="J24" s="133"/>
-      <c r="K24" s="134"/>
-      <c r="L24" s="134"/>
-      <c r="M24" s="135"/>
+      <c r="A24" s="135"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="143"/>
+      <c r="I24" s="136"/>
+      <c r="J24" s="135"/>
+      <c r="K24" s="143"/>
+      <c r="L24" s="143"/>
+      <c r="M24" s="136"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="136"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="137"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="137"/>
-      <c r="G25" s="137"/>
-      <c r="H25" s="137"/>
-      <c r="I25" s="138"/>
-      <c r="J25" s="136"/>
-      <c r="K25" s="137"/>
-      <c r="L25" s="137"/>
-      <c r="M25" s="138"/>
+      <c r="A25" s="132"/>
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="133"/>
+      <c r="H25" s="133"/>
+      <c r="I25" s="137"/>
+      <c r="J25" s="132"/>
+      <c r="K25" s="133"/>
+      <c r="L25" s="133"/>
+      <c r="M25" s="137"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="127" t="s">
+      <c r="A26" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="128"/>
-      <c r="C26" s="128"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="128"/>
-      <c r="J26" s="144"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="147"/>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
@@ -2169,39 +2171,39 @@
       <c r="L27" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="M27" s="132"/>
+      <c r="M27" s="134"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="136"/>
-      <c r="B28" s="137"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
-      <c r="H28" s="137"/>
-      <c r="I28" s="137"/>
-      <c r="J28" s="137"/>
+      <c r="A28" s="132"/>
+      <c r="B28" s="133"/>
+      <c r="C28" s="133"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="133"/>
+      <c r="G28" s="133"/>
+      <c r="H28" s="133"/>
+      <c r="I28" s="133"/>
+      <c r="J28" s="133"/>
       <c r="K28" s="23"/>
-      <c r="L28" s="133"/>
-      <c r="M28" s="135"/>
+      <c r="L28" s="135"/>
+      <c r="M28" s="136"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="127" t="s">
+      <c r="A29" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="128"/>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
-      <c r="J29" s="129"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="140"/>
       <c r="K29" s="23"/>
-      <c r="L29" s="133"/>
-      <c r="M29" s="135"/>
+      <c r="L29" s="135"/>
+      <c r="M29" s="136"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="130"/>
@@ -2215,23 +2217,23 @@
       <c r="I30" s="131"/>
       <c r="J30" s="131"/>
       <c r="K30" s="23"/>
-      <c r="L30" s="133"/>
-      <c r="M30" s="135"/>
+      <c r="L30" s="135"/>
+      <c r="M30" s="136"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="136"/>
-      <c r="B31" s="137"/>
-      <c r="C31" s="137"/>
-      <c r="D31" s="137"/>
-      <c r="E31" s="137"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="137"/>
-      <c r="I31" s="137"/>
-      <c r="J31" s="137"/>
+      <c r="A31" s="132"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="133"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="133"/>
+      <c r="H31" s="133"/>
+      <c r="I31" s="133"/>
+      <c r="J31" s="133"/>
       <c r="K31" s="23"/>
-      <c r="L31" s="136"/>
-      <c r="M31" s="138"/>
+      <c r="L31" s="132"/>
+      <c r="M31" s="137"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
@@ -2320,6 +2322,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A27:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="J7:M10"/>
+    <mergeCell ref="A7:C10"/>
+    <mergeCell ref="E7:H10"/>
     <mergeCell ref="A30:J31"/>
     <mergeCell ref="L27:M31"/>
     <mergeCell ref="A11:F11"/>
@@ -2335,15 +2346,6 @@
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A15:F18"/>
     <mergeCell ref="A26:J26"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A27:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="J7:M10"/>
-    <mergeCell ref="A7:C10"/>
-    <mergeCell ref="E7:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2376,187 +2378,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="155"/>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="108"/>
+      <c r="A1" s="152"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="100"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="13"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="100"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="16"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="100"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="16"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="100"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="16"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="153"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="154"/>
-      <c r="H6" s="154"/>
-      <c r="I6" s="100"/>
+      <c r="A6" s="150"/>
+      <c r="B6" s="151"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="17"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="157"/>
-      <c r="B7" s="158"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="164"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="169"/>
-      <c r="H7" s="170"/>
-      <c r="I7" s="100"/>
+      <c r="A7" s="154"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="166"/>
+      <c r="H7" s="167"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="16"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="160"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="169"/>
-      <c r="H8" s="170"/>
-      <c r="I8" s="100"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="157"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="166"/>
+      <c r="H8" s="167"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="16"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="159"/>
-      <c r="B9" s="160"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="169"/>
-      <c r="H9" s="170"/>
-      <c r="I9" s="100"/>
+      <c r="A9" s="156"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="166"/>
+      <c r="H9" s="167"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="16"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="159"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="170"/>
-      <c r="I10" s="100"/>
+      <c r="A10" s="156"/>
+      <c r="B10" s="157"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="166"/>
+      <c r="H10" s="167"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="16"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="17"/>
-      <c r="O10" s="85"/>
+      <c r="O10" s="32"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="168"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="170"/>
-      <c r="I11" s="100"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="164"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="166"/>
+      <c r="H11" s="167"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="16"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="17"/>
-      <c r="O11" s="86"/>
+      <c r="O11" s="33"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="1"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="145"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="100"/>
+      <c r="G12" s="168"/>
+      <c r="H12" s="169"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="17"/>
-      <c r="O12" s="86"/>
+      <c r="O12" s="33"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -2565,14 +2567,14 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="149"/>
-      <c r="H13" s="150"/>
-      <c r="I13" s="100"/>
+      <c r="G13" s="172"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="16"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="17"/>
-      <c r="O13" s="86"/>
+      <c r="O13" s="33"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -2581,14 +2583,14 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="100"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="16"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="86"/>
+      <c r="O14" s="33"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -2597,14 +2599,14 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="100"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="47"/>
       <c r="J15" s="16"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="17"/>
-      <c r="O15" s="86"/>
+      <c r="O15" s="33"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -2615,14 +2617,14 @@
         <v>9</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="100"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="16"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="17"/>
-      <c r="O16" s="86"/>
+      <c r="O16" s="33"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -2631,14 +2633,14 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="151"/>
-      <c r="H17" s="152"/>
-      <c r="I17" s="100"/>
+      <c r="G17" s="148"/>
+      <c r="H17" s="149"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="16"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="17"/>
-      <c r="O17" s="86"/>
+      <c r="O17" s="33"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
@@ -2647,14 +2649,14 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="100"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="16"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="17"/>
-      <c r="O18" s="87"/>
+      <c r="O18" s="34"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -2663,9 +2665,9 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="100"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="47"/>
       <c r="J19" s="16"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -2678,8 +2680,8 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="95"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
       <c r="I20" s="2"/>
       <c r="J20" s="16"/>
       <c r="K20" s="12"/>
@@ -2702,14 +2704,14 @@
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="96"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
       <c r="I22" s="11"/>
       <c r="J22" s="16"/>
       <c r="K22" s="12"/>
@@ -2717,14 +2719,14 @@
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
       <c r="I23" s="11"/>
       <c r="J23" s="16"/>
       <c r="K23" s="12"/>
@@ -2732,14 +2734,14 @@
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
+      <c r="A24" s="95"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="96"/>
       <c r="I24" s="11"/>
       <c r="J24" s="16"/>
       <c r="K24" s="12"/>
@@ -2747,14 +2749,14 @@
       <c r="M24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="96"/>
       <c r="I25" s="11"/>
       <c r="J25" s="16"/>
       <c r="K25" s="12"/>
@@ -2762,14 +2764,14 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
+      <c r="A26" s="95"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="96"/>
+      <c r="H26" s="96"/>
       <c r="I26" s="11"/>
       <c r="J26" s="16"/>
       <c r="K26" s="12"/>
@@ -2777,14 +2779,14 @@
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
-      <c r="B27" s="148"/>
-      <c r="C27" s="148"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
-      <c r="H27" s="148"/>
+      <c r="A27" s="170"/>
+      <c r="B27" s="171"/>
+      <c r="C27" s="171"/>
+      <c r="D27" s="171"/>
+      <c r="E27" s="171"/>
+      <c r="F27" s="171"/>
+      <c r="G27" s="171"/>
+      <c r="H27" s="171"/>
       <c r="I27" s="11"/>
       <c r="J27" s="16"/>
       <c r="K27" s="12"/>
@@ -2792,14 +2794,14 @@
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
       <c r="I28" s="11"/>
       <c r="J28" s="16"/>
       <c r="K28" s="12"/>
@@ -2807,14 +2809,14 @@
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="84"/>
       <c r="I29" s="11"/>
       <c r="J29" s="16"/>
       <c r="K29" s="12"/>
@@ -2822,14 +2824,14 @@
       <c r="M29" s="17"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="84"/>
       <c r="I30" s="11"/>
       <c r="J30" s="16"/>
       <c r="K30" s="12"/>
@@ -2837,14 +2839,14 @@
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="38"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
+      <c r="A31" s="83"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="84"/>
       <c r="I31" s="11"/>
       <c r="J31" s="16"/>
       <c r="K31" s="12"/>
@@ -2852,14 +2854,14 @@
       <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="84"/>
       <c r="I32" s="11"/>
       <c r="J32" s="16"/>
       <c r="K32" s="12"/>
@@ -2867,14 +2869,14 @@
       <c r="M32" s="17"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="38"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
       <c r="I33" s="11"/>
       <c r="J33" s="18"/>
       <c r="K33" s="19"/>
@@ -2883,13 +2885,21 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="31"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A22:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H33"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H16"/>
     <mergeCell ref="O10:O18"/>
     <mergeCell ref="G18:H20"/>
     <mergeCell ref="G17:H17"/>
@@ -2903,14 +2913,6 @@
     <mergeCell ref="A7:B11"/>
     <mergeCell ref="D7:E11"/>
     <mergeCell ref="G7:H11"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A22:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H33"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2982,23 +2984,23 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="171">
+      <c r="A3" s="174">
         <v>167</v>
       </c>
-      <c r="B3" s="171"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="171"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
       <c r="G3">
         <v>73</v>
       </c>
-      <c r="K3" s="171">
+      <c r="K3" s="174">
         <v>100</v>
       </c>
-      <c r="L3" s="171"/>
-      <c r="M3" s="171"/>
-      <c r="N3" s="171"/>
+      <c r="L3" s="174"/>
+      <c r="M3" s="174"/>
+      <c r="N3" s="174"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3118,123 +3120,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="173" t="s">
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="172"/>
-      <c r="N1" s="172"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="173" t="s">
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="172"/>
-      <c r="X1" s="172"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D2" s="175" t="s">
+      <c r="D2" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="175"/>
-      <c r="G2" s="176" t="s">
+      <c r="E2" s="176"/>
+      <c r="G2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="176" t="s">
+      <c r="I2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="177"/>
-      <c r="N2" s="175" t="s">
+      <c r="J2" s="31"/>
+      <c r="N2" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="175"/>
-      <c r="Q2" s="176" t="s">
+      <c r="O2" s="176"/>
+      <c r="Q2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="176" t="s">
+      <c r="S2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="177"/>
-      <c r="X2" s="175" t="s">
+      <c r="T2" s="31"/>
+      <c r="X2" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="175"/>
-      <c r="AA2" s="176" t="s">
+      <c r="Y2" s="176"/>
+      <c r="AA2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AC2" s="176" t="s">
+      <c r="AC2" s="30" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="174"/>
-      <c r="B3" s="174"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="G3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="177"/>
-      <c r="K3" s="174"/>
-      <c r="L3" s="174"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="Q3" s="176"/>
-      <c r="S3" s="176"/>
-      <c r="T3" s="177"/>
-      <c r="U3" s="174"/>
-      <c r="V3" s="174"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="AA3" s="176"/>
-      <c r="AC3" s="176"/>
+      <c r="A3" s="175"/>
+      <c r="B3" s="175"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="G3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="175"/>
+      <c r="L3" s="175"/>
+      <c r="N3" s="176"/>
+      <c r="O3" s="176"/>
+      <c r="Q3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="X3" s="176"/>
+      <c r="Y3" s="176"/>
+      <c r="AA3" s="30"/>
+      <c r="AC3" s="30"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="174"/>
-      <c r="B4" s="174"/>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175"/>
-      <c r="G4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="174"/>
-      <c r="L4" s="174"/>
-      <c r="N4" s="175"/>
-      <c r="O4" s="175"/>
-      <c r="Q4" s="176"/>
-      <c r="S4" s="176"/>
-      <c r="T4" s="177"/>
-      <c r="U4" s="174"/>
-      <c r="V4" s="174"/>
-      <c r="X4" s="175"/>
-      <c r="Y4" s="175"/>
-      <c r="AA4" s="176"/>
-      <c r="AC4" s="176"/>
+      <c r="A4" s="175"/>
+      <c r="B4" s="175"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="G4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="175"/>
+      <c r="L4" s="175"/>
+      <c r="N4" s="176"/>
+      <c r="O4" s="176"/>
+      <c r="Q4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="175"/>
+      <c r="V4" s="175"/>
+      <c r="X4" s="176"/>
+      <c r="Y4" s="176"/>
+      <c r="AA4" s="30"/>
+      <c r="AC4" s="30"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="174"/>
-      <c r="B5" s="174"/>
-      <c r="D5" s="175"/>
-      <c r="E5" s="175"/>
-      <c r="G5" s="176"/>
-      <c r="I5" s="176"/>
-      <c r="J5" s="177"/>
-      <c r="K5" s="174"/>
-      <c r="L5" s="174"/>
-      <c r="N5" s="175"/>
-      <c r="O5" s="175"/>
-      <c r="Q5" s="176"/>
-      <c r="S5" s="176"/>
-      <c r="T5" s="177"/>
-      <c r="U5" s="174"/>
-      <c r="V5" s="174"/>
-      <c r="X5" s="175"/>
-      <c r="Y5" s="175"/>
-      <c r="AA5" s="176"/>
-      <c r="AC5" s="176"/>
+      <c r="A5" s="175"/>
+      <c r="B5" s="175"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="G5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="175"/>
+      <c r="L5" s="175"/>
+      <c r="N5" s="176"/>
+      <c r="O5" s="176"/>
+      <c r="Q5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="175"/>
+      <c r="V5" s="175"/>
+      <c r="X5" s="176"/>
+      <c r="Y5" s="176"/>
+      <c r="AA5" s="30"/>
+      <c r="AC5" s="30"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3421,6 +3423,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="W1:X1"/>
@@ -3437,14 +3447,6 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3454,7 +3456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3497,4 +3499,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="178"/>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="178"/>
+      <c r="E6" s="178"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="178"/>
+      <c r="E8" s="178"/>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="178"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="178"/>
+      <c r="E11" s="178"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="178"/>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="178"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fin nom cabinet / debut PNJ
</commit_message>
<xml_diff>
--- a/Cabinet des murmures/ressources/Cabinet schema.xlsx
+++ b/Cabinet des murmures/ressources/Cabinet schema.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cabinet" sheetId="1" r:id="rId1"/>
     <sheet name="Esprit" sheetId="2" r:id="rId2"/>
     <sheet name="Corps" sheetId="4" r:id="rId3"/>
-    <sheet name="Arme" sheetId="5" r:id="rId4"/>
-    <sheet name="pouvoir" sheetId="6" r:id="rId5"/>
-    <sheet name="perisprit" sheetId="7" r:id="rId6"/>
-    <sheet name="arbre" sheetId="8" r:id="rId7"/>
+    <sheet name="PNJ" sheetId="9" r:id="rId4"/>
+    <sheet name="Arme" sheetId="5" r:id="rId5"/>
+    <sheet name="pouvoir" sheetId="6" r:id="rId6"/>
+    <sheet name="perisprit" sheetId="7" r:id="rId7"/>
+    <sheet name="arbre" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>XP</t>
   </si>
@@ -93,6 +94,33 @@
   <si>
     <t>C.</t>
   </si>
+  <si>
+    <t>Attributs</t>
+  </si>
+  <si>
+    <t>Sante</t>
+  </si>
+  <si>
+    <t>Energie</t>
+  </si>
+  <si>
+    <t>Perisprit</t>
+  </si>
+  <si>
+    <t>Pouvoir</t>
+  </si>
+  <si>
+    <t>et Corruptions</t>
+  </si>
+  <si>
+    <t>Armes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Combat</t>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,8 +299,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -449,11 +483,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +553,178 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,173 +851,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -804,42 +866,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,6 +905,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -912,24 +983,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,7 +995,49 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,419 +1361,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="50"/>
+      <c r="A1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="108"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="67"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="70"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="128"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70"/>
+      <c r="A4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="102"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="128"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="70"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="128"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="70"/>
+      <c r="A7" s="114"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="128"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="70"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="128"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="70"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="128"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="70"/>
-      <c r="L10" s="32"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="128"/>
+      <c r="L10" s="90"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="70"/>
-      <c r="L11" s="33"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="127"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="128"/>
+      <c r="L11" s="91"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="73"/>
-      <c r="L12" s="33"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="129"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="131"/>
+      <c r="L12" s="91"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="103"/>
-      <c r="L13" s="33"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
+      <c r="L13" s="91"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="80"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="106"/>
-      <c r="L14" s="33"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="66"/>
+      <c r="L14" s="91"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="85"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="109"/>
-      <c r="L15" s="33"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="69"/>
+      <c r="L15" s="91"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="109"/>
-      <c r="L16" s="33"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="69"/>
+      <c r="L16" s="91"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="109"/>
-      <c r="L17" s="33"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="69"/>
+      <c r="L17" s="91"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="109"/>
-      <c r="L18" s="33"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="69"/>
+      <c r="L18" s="91"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="83"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="109"/>
-      <c r="L19" s="34"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="69"/>
+      <c r="L19" s="92"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="87"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="110"/>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="112"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="72"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="89"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="91"/>
-      <c r="H21" s="127"/>
-      <c r="I21" s="113"/>
-      <c r="J21" s="114"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="87"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="74"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="127"/>
-      <c r="I22" s="115"/>
-      <c r="J22" s="116"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="76"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="95"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="127"/>
-      <c r="I23" s="117"/>
-      <c r="J23" s="118"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="78"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="97"/>
-      <c r="H24" s="127"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="118"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="78"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="117"/>
-      <c r="J25" s="118"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="78"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="96"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="117"/>
-      <c r="J26" s="118"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="78"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="95"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="127"/>
-      <c r="I27" s="119"/>
-      <c r="J27" s="120"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="80"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="128"/>
-      <c r="J28" s="128"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="95"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="96"/>
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="127"/>
-      <c r="I29" s="129"/>
-      <c r="J29" s="129"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="89"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="95"/>
-      <c r="B30" s="96"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="96"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="127"/>
-      <c r="I30" s="121"/>
-      <c r="J30" s="122"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="82"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="95"/>
-      <c r="B31" s="96"/>
-      <c r="C31" s="96"/>
-      <c r="D31" s="96"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="127"/>
-      <c r="I31" s="123"/>
-      <c r="J31" s="124"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="87"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="84"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="95"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="127"/>
-      <c r="I32" s="123"/>
-      <c r="J32" s="124"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="84"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="98"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="127"/>
-      <c r="I33" s="125"/>
-      <c r="J33" s="126"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="87"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="86"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="74"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="76"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="L10:L19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E5"/>
+    <mergeCell ref="F1:F20"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="G2:J12"/>
+    <mergeCell ref="B7:B12"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E20"/>
@@ -1691,18 +1798,6 @@
     <mergeCell ref="I30:J33"/>
     <mergeCell ref="H21:H33"/>
     <mergeCell ref="I28:J29"/>
-    <mergeCell ref="L10:L19"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E5"/>
-    <mergeCell ref="F1:F20"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="G2:J12"/>
-    <mergeCell ref="B7:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1733,507 +1828,507 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="140"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="134"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="130"/>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="134"/>
+      <c r="A2" s="135"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="137"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="135"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="136"/>
+      <c r="A3" s="138"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="140"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="135"/>
-      <c r="B4" s="143"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="143"/>
-      <c r="K4" s="143"/>
-      <c r="L4" s="143"/>
-      <c r="M4" s="136"/>
+      <c r="A4" s="138"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="140"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="132"/>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133"/>
-      <c r="M5" s="137"/>
+      <c r="A5" s="141"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="142"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="142"/>
+      <c r="M5" s="143"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="138" t="s">
+      <c r="A6" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="139"/>
-      <c r="C6" s="140"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="134"/>
       <c r="D6" s="24"/>
-      <c r="E6" s="138" t="s">
+      <c r="E6" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="139"/>
-      <c r="G6" s="139"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="139"/>
-      <c r="L6" s="139"/>
-      <c r="M6" s="140"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="133"/>
+      <c r="J6" s="133"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="134"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="130"/>
-      <c r="B7" s="131"/>
-      <c r="C7" s="134"/>
+      <c r="A7" s="135"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="137"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="136"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="140"/>
       <c r="I7" s="24"/>
-      <c r="J7" s="135"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="136"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="140"/>
       <c r="O7" s="26"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="135"/>
-      <c r="B8" s="143"/>
-      <c r="C8" s="136"/>
+      <c r="A8" s="138"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="140"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="136"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="140"/>
       <c r="I8" s="24"/>
-      <c r="J8" s="135"/>
-      <c r="K8" s="143"/>
-      <c r="L8" s="143"/>
-      <c r="M8" s="136"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="139"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="140"/>
       <c r="O8" s="27"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="143"/>
-      <c r="C9" s="136"/>
+      <c r="A9" s="138"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="140"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="135"/>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="136"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="140"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="135"/>
-      <c r="K9" s="143"/>
-      <c r="L9" s="143"/>
-      <c r="M9" s="136"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="140"/>
       <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="135"/>
-      <c r="B10" s="143"/>
-      <c r="C10" s="136"/>
+      <c r="A10" s="138"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="140"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="136"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="140"/>
       <c r="I10" s="24"/>
-      <c r="J10" s="135"/>
-      <c r="K10" s="143"/>
-      <c r="L10" s="143"/>
-      <c r="M10" s="136"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="139"/>
+      <c r="M10" s="140"/>
       <c r="O10" s="27"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="139"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="139"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="140"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="134"/>
       <c r="G11" s="24"/>
-      <c r="H11" s="138" t="s">
+      <c r="H11" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="139"/>
-      <c r="J11" s="139"/>
-      <c r="K11" s="139"/>
-      <c r="L11" s="139"/>
-      <c r="M11" s="140"/>
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="134"/>
       <c r="O11" s="27"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="134"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="137"/>
       <c r="G12" s="24"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="134"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="136"/>
+      <c r="J12" s="136"/>
+      <c r="K12" s="136"/>
+      <c r="L12" s="136"/>
+      <c r="M12" s="137"/>
       <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="135"/>
-      <c r="B13" s="143"/>
-      <c r="C13" s="143"/>
-      <c r="D13" s="143"/>
-      <c r="E13" s="143"/>
-      <c r="F13" s="136"/>
+      <c r="A13" s="138"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="140"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="135"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="143"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="143"/>
-      <c r="M13" s="136"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="139"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="140"/>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="145"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="146"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="147"/>
+      <c r="D14" s="147"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="148"/>
       <c r="G14" s="24"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="137"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="142"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="142"/>
+      <c r="L14" s="142"/>
+      <c r="M14" s="143"/>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="130"/>
-      <c r="B15" s="131"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="134"/>
+      <c r="A15" s="135"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
+      <c r="F15" s="137"/>
       <c r="G15" s="25"/>
-      <c r="H15" s="138" t="s">
+      <c r="H15" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="139"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="139"/>
-      <c r="L15" s="139"/>
-      <c r="M15" s="140"/>
+      <c r="I15" s="133"/>
+      <c r="J15" s="133"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="133"/>
+      <c r="M15" s="134"/>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="135"/>
-      <c r="B16" s="143"/>
-      <c r="C16" s="143"/>
-      <c r="D16" s="143"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="136"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="140"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="131"/>
-      <c r="L16" s="131"/>
-      <c r="M16" s="134"/>
+      <c r="H16" s="135"/>
+      <c r="I16" s="136"/>
+      <c r="J16" s="136"/>
+      <c r="K16" s="136"/>
+      <c r="L16" s="136"/>
+      <c r="M16" s="137"/>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="135"/>
-      <c r="B17" s="143"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="143"/>
-      <c r="E17" s="143"/>
-      <c r="F17" s="136"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="140"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="143"/>
-      <c r="J17" s="143"/>
-      <c r="K17" s="143"/>
-      <c r="L17" s="143"/>
-      <c r="M17" s="136"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="139"/>
+      <c r="K17" s="139"/>
+      <c r="L17" s="139"/>
+      <c r="M17" s="140"/>
       <c r="O17" s="27"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="132"/>
-      <c r="B18" s="133"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="133"/>
-      <c r="F18" s="137"/>
+      <c r="A18" s="141"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="143"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="136"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="139"/>
+      <c r="K18" s="139"/>
+      <c r="L18" s="139"/>
+      <c r="M18" s="140"/>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="141" t="s">
+      <c r="A19" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="142"/>
-      <c r="C19" s="142"/>
-      <c r="D19" s="142"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="139"/>
-      <c r="H19" s="139"/>
-      <c r="I19" s="139"/>
-      <c r="J19" s="139"/>
-      <c r="K19" s="139"/>
-      <c r="L19" s="139"/>
-      <c r="M19" s="140"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="145"/>
+      <c r="E19" s="145"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="133"/>
+      <c r="J19" s="133"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="133"/>
+      <c r="M19" s="134"/>
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="130"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="131"/>
-      <c r="G20" s="131"/>
-      <c r="H20" s="131"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="130"/>
-      <c r="K20" s="131"/>
-      <c r="L20" s="131"/>
-      <c r="M20" s="134"/>
+      <c r="A20" s="135"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="135"/>
+      <c r="K20" s="136"/>
+      <c r="L20" s="136"/>
+      <c r="M20" s="137"/>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="135"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="143"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="143"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="143"/>
-      <c r="I21" s="136"/>
-      <c r="J21" s="135"/>
-      <c r="K21" s="143"/>
-      <c r="L21" s="143"/>
-      <c r="M21" s="136"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="139"/>
+      <c r="I21" s="140"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="139"/>
+      <c r="L21" s="139"/>
+      <c r="M21" s="140"/>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="135"/>
-      <c r="B22" s="143"/>
-      <c r="C22" s="143"/>
-      <c r="D22" s="136"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="143"/>
-      <c r="G22" s="143"/>
-      <c r="H22" s="143"/>
-      <c r="I22" s="136"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="143"/>
-      <c r="L22" s="143"/>
-      <c r="M22" s="136"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="140"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="140"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="139"/>
+      <c r="L22" s="139"/>
+      <c r="M22" s="140"/>
       <c r="O22" s="28"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="135"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="135"/>
-      <c r="F23" s="143"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="136"/>
-      <c r="J23" s="135"/>
-      <c r="K23" s="143"/>
-      <c r="L23" s="143"/>
-      <c r="M23" s="136"/>
+      <c r="A23" s="138"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="140"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="139"/>
+      <c r="I23" s="140"/>
+      <c r="J23" s="138"/>
+      <c r="K23" s="139"/>
+      <c r="L23" s="139"/>
+      <c r="M23" s="140"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="135"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="136"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="143"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="136"/>
-      <c r="J24" s="135"/>
-      <c r="K24" s="143"/>
-      <c r="L24" s="143"/>
-      <c r="M24" s="136"/>
+      <c r="A24" s="138"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="140"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="139"/>
+      <c r="I24" s="140"/>
+      <c r="J24" s="138"/>
+      <c r="K24" s="139"/>
+      <c r="L24" s="139"/>
+      <c r="M24" s="140"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="132"/>
-      <c r="B25" s="133"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="133"/>
-      <c r="G25" s="133"/>
-      <c r="H25" s="133"/>
-      <c r="I25" s="137"/>
-      <c r="J25" s="132"/>
-      <c r="K25" s="133"/>
-      <c r="L25" s="133"/>
-      <c r="M25" s="137"/>
+      <c r="A25" s="141"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="142"/>
+      <c r="D25" s="143"/>
+      <c r="E25" s="141"/>
+      <c r="F25" s="142"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="142"/>
+      <c r="I25" s="143"/>
+      <c r="J25" s="141"/>
+      <c r="K25" s="142"/>
+      <c r="L25" s="142"/>
+      <c r="M25" s="143"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="138" t="s">
+      <c r="A26" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="139"/>
-      <c r="C26" s="139"/>
-      <c r="D26" s="139"/>
-      <c r="E26" s="139"/>
-      <c r="F26" s="139"/>
-      <c r="G26" s="139"/>
-      <c r="H26" s="139"/>
-      <c r="I26" s="139"/>
-      <c r="J26" s="147"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="133"/>
+      <c r="G26" s="133"/>
+      <c r="H26" s="133"/>
+      <c r="I26" s="133"/>
+      <c r="J26" s="149"/>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="130"/>
-      <c r="B27" s="131"/>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="131"/>
+      <c r="A27" s="135"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="136"/>
+      <c r="J27" s="136"/>
       <c r="K27" s="23"/>
-      <c r="L27" s="130" t="s">
+      <c r="L27" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="M27" s="134"/>
+      <c r="M27" s="137"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="132"/>
-      <c r="B28" s="133"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
-      <c r="F28" s="133"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="133"/>
-      <c r="J28" s="133"/>
+      <c r="A28" s="141"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="142"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="142"/>
       <c r="K28" s="23"/>
-      <c r="L28" s="135"/>
-      <c r="M28" s="136"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="140"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="138" t="s">
+      <c r="A29" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="139"/>
-      <c r="C29" s="139"/>
-      <c r="D29" s="139"/>
-      <c r="E29" s="139"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="139"/>
-      <c r="I29" s="139"/>
-      <c r="J29" s="140"/>
+      <c r="B29" s="133"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="133"/>
+      <c r="F29" s="133"/>
+      <c r="G29" s="133"/>
+      <c r="H29" s="133"/>
+      <c r="I29" s="133"/>
+      <c r="J29" s="134"/>
       <c r="K29" s="23"/>
-      <c r="L29" s="135"/>
-      <c r="M29" s="136"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="140"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="130"/>
-      <c r="B30" s="131"/>
-      <c r="C30" s="131"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="131"/>
-      <c r="F30" s="131"/>
-      <c r="G30" s="131"/>
-      <c r="H30" s="131"/>
-      <c r="I30" s="131"/>
-      <c r="J30" s="131"/>
+      <c r="A30" s="135"/>
+      <c r="B30" s="136"/>
+      <c r="C30" s="136"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="136"/>
+      <c r="J30" s="136"/>
       <c r="K30" s="23"/>
-      <c r="L30" s="135"/>
-      <c r="M30" s="136"/>
+      <c r="L30" s="138"/>
+      <c r="M30" s="140"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="132"/>
-      <c r="B31" s="133"/>
-      <c r="C31" s="133"/>
-      <c r="D31" s="133"/>
-      <c r="E31" s="133"/>
-      <c r="F31" s="133"/>
-      <c r="G31" s="133"/>
-      <c r="H31" s="133"/>
-      <c r="I31" s="133"/>
-      <c r="J31" s="133"/>
+      <c r="A31" s="141"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="142"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="142"/>
+      <c r="I31" s="142"/>
+      <c r="J31" s="142"/>
       <c r="K31" s="23"/>
-      <c r="L31" s="132"/>
-      <c r="M31" s="137"/>
+      <c r="L31" s="141"/>
+      <c r="M31" s="143"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
@@ -2322,15 +2417,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A27:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="J7:M10"/>
-    <mergeCell ref="A7:C10"/>
-    <mergeCell ref="E7:H10"/>
     <mergeCell ref="A30:J31"/>
     <mergeCell ref="L27:M31"/>
     <mergeCell ref="A11:F11"/>
@@ -2346,6 +2432,15 @@
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A15:F18"/>
     <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A27:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="J7:M10"/>
+    <mergeCell ref="A7:C10"/>
+    <mergeCell ref="E7:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2378,187 +2473,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="152"/>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55"/>
+      <c r="A1" s="160"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="113"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="47"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="105"/>
       <c r="J2" s="13"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="47"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="105"/>
       <c r="J3" s="16"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="47"/>
+      <c r="A4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="105"/>
       <c r="J4" s="16"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="47"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="105"/>
       <c r="J5" s="16"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="150"/>
-      <c r="B6" s="151"/>
-      <c r="C6" s="151"/>
-      <c r="D6" s="151"/>
-      <c r="E6" s="151"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="151"/>
-      <c r="I6" s="47"/>
+      <c r="A6" s="158"/>
+      <c r="B6" s="159"/>
+      <c r="C6" s="159"/>
+      <c r="D6" s="159"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="159"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="159"/>
+      <c r="I6" s="105"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="17"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="154"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="160"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="166"/>
-      <c r="H7" s="167"/>
-      <c r="I7" s="47"/>
+      <c r="A7" s="162"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="168"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="174"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="105"/>
       <c r="J7" s="16"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="156"/>
-      <c r="B8" s="157"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="162"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="166"/>
-      <c r="H8" s="167"/>
-      <c r="I8" s="47"/>
+      <c r="A8" s="164"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="171"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="105"/>
       <c r="J8" s="16"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="156"/>
-      <c r="B9" s="157"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="162"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="166"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="47"/>
+      <c r="A9" s="164"/>
+      <c r="B9" s="165"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="175"/>
+      <c r="I9" s="105"/>
       <c r="J9" s="16"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="156"/>
-      <c r="B10" s="157"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="167"/>
-      <c r="I10" s="47"/>
+      <c r="A10" s="164"/>
+      <c r="B10" s="165"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="174"/>
+      <c r="H10" s="175"/>
+      <c r="I10" s="105"/>
       <c r="J10" s="16"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="17"/>
-      <c r="O10" s="32"/>
+      <c r="O10" s="90"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="158"/>
-      <c r="B11" s="159"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="164"/>
-      <c r="E11" s="165"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="166"/>
-      <c r="H11" s="167"/>
-      <c r="I11" s="47"/>
+      <c r="A11" s="166"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="174"/>
+      <c r="H11" s="175"/>
+      <c r="I11" s="105"/>
       <c r="J11" s="16"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="17"/>
-      <c r="O11" s="33"/>
+      <c r="O11" s="91"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="77"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="1"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="168"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="47"/>
+      <c r="G12" s="150"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="105"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="17"/>
-      <c r="O12" s="33"/>
+      <c r="O12" s="91"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -2567,14 +2662,14 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="172"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="47"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="155"/>
+      <c r="I13" s="105"/>
       <c r="J13" s="16"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="17"/>
-      <c r="O13" s="33"/>
+      <c r="O13" s="91"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -2583,14 +2678,14 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="108"/>
-      <c r="I14" s="47"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="105"/>
       <c r="J14" s="16"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="17"/>
-      <c r="O14" s="33"/>
+      <c r="O14" s="91"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -2599,14 +2694,14 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="47"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="105"/>
       <c r="J15" s="16"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="17"/>
-      <c r="O15" s="33"/>
+      <c r="O15" s="91"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -2617,14 +2712,14 @@
         <v>9</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="47"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="105"/>
       <c r="J16" s="16"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="17"/>
-      <c r="O16" s="33"/>
+      <c r="O16" s="91"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -2633,14 +2728,14 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="148"/>
-      <c r="H17" s="149"/>
-      <c r="I17" s="47"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="105"/>
       <c r="J17" s="16"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="17"/>
-      <c r="O17" s="33"/>
+      <c r="O17" s="91"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
@@ -2649,14 +2744,14 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="47"/>
+      <c r="G18" s="99"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="105"/>
       <c r="J18" s="16"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="17"/>
-      <c r="O18" s="34"/>
+      <c r="O18" s="92"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -2665,9 +2760,9 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="47"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="105"/>
       <c r="J19" s="16"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -2680,8 +2775,8 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="100"/>
       <c r="I20" s="2"/>
       <c r="J20" s="16"/>
       <c r="K20" s="12"/>
@@ -2704,14 +2799,14 @@
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
       <c r="I22" s="11"/>
       <c r="J22" s="16"/>
       <c r="K22" s="12"/>
@@ -2719,14 +2814,14 @@
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="95"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
       <c r="I23" s="11"/>
       <c r="J23" s="16"/>
       <c r="K23" s="12"/>
@@ -2734,14 +2829,14 @@
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="95"/>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="96"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="11"/>
       <c r="J24" s="16"/>
       <c r="K24" s="12"/>
@@ -2749,14 +2844,14 @@
       <c r="M24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="96"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="11"/>
       <c r="J25" s="16"/>
       <c r="K25" s="12"/>
@@ -2764,14 +2859,14 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="96"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="96"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="11"/>
       <c r="J26" s="16"/>
       <c r="K26" s="12"/>
@@ -2779,14 +2874,14 @@
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="170"/>
-      <c r="B27" s="171"/>
-      <c r="C27" s="171"/>
-      <c r="D27" s="171"/>
-      <c r="E27" s="171"/>
-      <c r="F27" s="171"/>
-      <c r="G27" s="171"/>
-      <c r="H27" s="171"/>
+      <c r="A27" s="152"/>
+      <c r="B27" s="153"/>
+      <c r="C27" s="153"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="153"/>
       <c r="I27" s="11"/>
       <c r="J27" s="16"/>
       <c r="K27" s="12"/>
@@ -2794,14 +2889,14 @@
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="83"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
       <c r="I28" s="11"/>
       <c r="J28" s="16"/>
       <c r="K28" s="12"/>
@@ -2809,14 +2904,14 @@
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
       <c r="I29" s="11"/>
       <c r="J29" s="16"/>
       <c r="K29" s="12"/>
@@ -2824,14 +2919,14 @@
       <c r="M29" s="17"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
       <c r="I30" s="11"/>
       <c r="J30" s="16"/>
       <c r="K30" s="12"/>
@@ -2839,14 +2934,14 @@
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
-      <c r="G31" s="84"/>
-      <c r="H31" s="84"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
       <c r="I31" s="11"/>
       <c r="J31" s="16"/>
       <c r="K31" s="12"/>
@@ -2854,14 +2949,14 @@
       <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="84"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
       <c r="I32" s="11"/>
       <c r="J32" s="16"/>
       <c r="K32" s="12"/>
@@ -2869,14 +2964,14 @@
       <c r="M32" s="17"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
       <c r="I33" s="11"/>
       <c r="J33" s="18"/>
       <c r="K33" s="19"/>
@@ -2885,21 +2980,13 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="74"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="76"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="A22:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H33"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H16"/>
     <mergeCell ref="O10:O18"/>
     <mergeCell ref="G18:H20"/>
     <mergeCell ref="G17:H17"/>
@@ -2913,6 +3000,14 @@
     <mergeCell ref="A7:B11"/>
     <mergeCell ref="D7:E11"/>
     <mergeCell ref="G7:H11"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A22:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H33"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2920,6 +3015,294 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="198" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="182"/>
+      <c r="D6" s="199" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="200"/>
+      <c r="F6" s="201"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="109"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="109"/>
+      <c r="F7" s="183"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="110"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="110"/>
+      <c r="F8" s="184"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="110"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="110"/>
+      <c r="F9" s="184"/>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="180"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="110"/>
+      <c r="F10" s="184"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="202" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="199" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="200"/>
+      <c r="F11" s="201"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="109"/>
+      <c r="D12" s="185"/>
+      <c r="E12" s="186"/>
+      <c r="F12" s="187"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="110"/>
+      <c r="D13" s="182"/>
+      <c r="E13" s="188"/>
+      <c r="F13" s="189"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="110"/>
+      <c r="D14" s="182"/>
+      <c r="E14" s="188"/>
+      <c r="F14" s="189"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="110"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="188"/>
+      <c r="F15" s="189"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="110"/>
+      <c r="D16" s="182"/>
+      <c r="E16" s="188"/>
+      <c r="F16" s="189"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="180"/>
+      <c r="D17" s="182"/>
+      <c r="E17" s="188"/>
+      <c r="F17" s="189"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="198" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="182"/>
+      <c r="E18" s="188"/>
+      <c r="F18" s="189"/>
+    </row>
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="181"/>
+      <c r="D19" s="182"/>
+      <c r="E19" s="188"/>
+      <c r="F19" s="189"/>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="198" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="182"/>
+      <c r="E20" s="188"/>
+      <c r="F20" s="189"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="181"/>
+      <c r="D21" s="182"/>
+      <c r="E21" s="188"/>
+      <c r="F21" s="189"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="198" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="182"/>
+      <c r="E22" s="188"/>
+      <c r="F22" s="189"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="109"/>
+      <c r="D23" s="182"/>
+      <c r="E23" s="188"/>
+      <c r="F23" s="189"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="180"/>
+      <c r="D24" s="182"/>
+      <c r="E24" s="188"/>
+      <c r="F24" s="189"/>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="198" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="190"/>
+      <c r="E25" s="191"/>
+      <c r="F25" s="192"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="198" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="199" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="200"/>
+      <c r="F26" s="201"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="109"/>
+      <c r="D27" s="193"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="194"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="110"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="105"/>
+      <c r="F28" s="195"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="110"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="195"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="110"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="105"/>
+      <c r="F30" s="195"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="110"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="195"/>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="110"/>
+      <c r="D32" s="196"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="197"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="199" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="200"/>
+      <c r="D33" s="200"/>
+      <c r="E33" s="200"/>
+      <c r="F33" s="201"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="193"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+      <c r="F34" s="194"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="87"/>
+      <c r="C35" s="105"/>
+      <c r="D35" s="105"/>
+      <c r="E35" s="105"/>
+      <c r="F35" s="195"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="87"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="195"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="196"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="197"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="199" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="200"/>
+      <c r="D38" s="200"/>
+      <c r="E38" s="200"/>
+      <c r="F38" s="201"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="193"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="194"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="87"/>
+      <c r="C40" s="105"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="195"/>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="196"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="197"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F41"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F32"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B23:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -2984,23 +3367,23 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="174">
+      <c r="A3" s="176">
         <v>167</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
+      <c r="F3" s="176"/>
       <c r="G3">
         <v>73</v>
       </c>
-      <c r="K3" s="174">
+      <c r="K3" s="176">
         <v>100</v>
       </c>
-      <c r="L3" s="174"/>
-      <c r="M3" s="174"/>
-      <c r="N3" s="174"/>
+      <c r="L3" s="176"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="176"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3081,7 +3464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC16"/>
   <sheetViews>
@@ -3123,26 +3506,26 @@
       <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
       <c r="J1" s="31"/>
       <c r="K1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
       <c r="T1" s="31"/>
       <c r="U1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D2" s="176" t="s">
+      <c r="D2" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="176"/>
+      <c r="E2" s="178"/>
       <c r="G2" s="30" t="s">
         <v>22</v>
       </c>
@@ -3150,10 +3533,10 @@
         <v>23</v>
       </c>
       <c r="J2" s="31"/>
-      <c r="N2" s="176" t="s">
+      <c r="N2" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="176"/>
+      <c r="O2" s="178"/>
       <c r="Q2" s="30" t="s">
         <v>22</v>
       </c>
@@ -3161,10 +3544,10 @@
         <v>23</v>
       </c>
       <c r="T2" s="31"/>
-      <c r="X2" s="176" t="s">
+      <c r="X2" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="176"/>
+      <c r="Y2" s="178"/>
       <c r="AA2" s="30" t="s">
         <v>22</v>
       </c>
@@ -3173,68 +3556,68 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="175"/>
-      <c r="B3" s="175"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
+      <c r="A3" s="177"/>
+      <c r="B3" s="177"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
       <c r="G3" s="30"/>
       <c r="I3" s="30"/>
       <c r="J3" s="31"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="175"/>
-      <c r="N3" s="176"/>
-      <c r="O3" s="176"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
+      <c r="N3" s="178"/>
+      <c r="O3" s="178"/>
       <c r="Q3" s="30"/>
       <c r="S3" s="30"/>
       <c r="T3" s="31"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="X3" s="176"/>
-      <c r="Y3" s="176"/>
+      <c r="U3" s="177"/>
+      <c r="V3" s="177"/>
+      <c r="X3" s="178"/>
+      <c r="Y3" s="178"/>
       <c r="AA3" s="30"/>
       <c r="AC3" s="30"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="175"/>
-      <c r="B4" s="175"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
+      <c r="A4" s="177"/>
+      <c r="B4" s="177"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
       <c r="G4" s="30"/>
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
-      <c r="K4" s="175"/>
-      <c r="L4" s="175"/>
-      <c r="N4" s="176"/>
-      <c r="O4" s="176"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
       <c r="Q4" s="30"/>
       <c r="S4" s="30"/>
       <c r="T4" s="31"/>
-      <c r="U4" s="175"/>
-      <c r="V4" s="175"/>
-      <c r="X4" s="176"/>
-      <c r="Y4" s="176"/>
+      <c r="U4" s="177"/>
+      <c r="V4" s="177"/>
+      <c r="X4" s="178"/>
+      <c r="Y4" s="178"/>
       <c r="AA4" s="30"/>
       <c r="AC4" s="30"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="175"/>
-      <c r="B5" s="175"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="176"/>
+      <c r="A5" s="177"/>
+      <c r="B5" s="177"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
       <c r="G5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="175"/>
-      <c r="L5" s="175"/>
-      <c r="N5" s="176"/>
-      <c r="O5" s="176"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="N5" s="178"/>
+      <c r="O5" s="178"/>
       <c r="Q5" s="30"/>
       <c r="S5" s="30"/>
       <c r="T5" s="31"/>
-      <c r="U5" s="175"/>
-      <c r="V5" s="175"/>
-      <c r="X5" s="176"/>
-      <c r="Y5" s="176"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="X5" s="178"/>
+      <c r="Y5" s="178"/>
       <c r="AA5" s="30"/>
       <c r="AC5" s="30"/>
     </row>
@@ -3423,14 +3806,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="W1:X1"/>
@@ -3447,12 +3822,20 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J18"/>
   <sheetViews>
@@ -3501,39 +3884,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D4" s="178"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="178"/>
-      <c r="E6" s="178"/>
+      <c r="C6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="178"/>
-      <c r="E8" s="178"/>
+      <c r="C8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="178"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="178"/>
-      <c r="E11" s="178"/>
+      <c r="C11" s="33"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="178"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="178"/>
+      <c r="D14" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>